<commit_message>
cganged no. of addresses to 2000
</commit_message>
<xml_diff>
--- a/docs/bangalore_dispatch_address_finals.xlsx
+++ b/docs/bangalore_dispatch_address_finals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Pavan\Projects\Growsimple\backend\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB65FC0-65CD-47DC-B4DA-DA81F4CD52DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4378734E-AC00-4C01-AB9F-740DA3CA7F3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8001" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8005" uniqueCount="549">
   <si>
     <t>address</t>
   </si>
@@ -2968,10 +2968,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2189"/>
+  <dimension ref="A1:E2001"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1549" workbookViewId="0">
-      <selection activeCell="C2003" sqref="C2003"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1985" workbookViewId="0">
+      <selection activeCell="E2000" sqref="E2000"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3060,7 +3060,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="6">
-        <f t="shared" ref="C5:C19" si="0">C3+4</f>
+        <f t="shared" ref="C5:C18" si="0">C3+4</f>
         <v>62201852043</v>
       </c>
       <c r="D5" s="5" t="s">
@@ -37890,7 +37890,7 @@
         <v>435</v>
       </c>
       <c r="C1940" s="6">
-        <f t="shared" ref="C1940:C2000" si="31">C1938+4</f>
+        <f t="shared" ref="C1940:C2001" si="31">C1938+4</f>
         <v>62201855914</v>
       </c>
       <c r="D1940" s="5" t="s">
@@ -38981,1327 +38981,22 @@
       </c>
     </row>
     <row r="2001" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2001" s="5"/>
-      <c r="B2001" s="5"/>
-      <c r="C2001" s="6"/>
-      <c r="D2001" s="5"/>
-      <c r="E2001" s="5"/>
-    </row>
-    <row r="2002" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2002" s="5"/>
-      <c r="B2002" s="5"/>
-      <c r="C2002" s="6"/>
-      <c r="D2002" s="5"/>
-      <c r="E2002" s="5"/>
-    </row>
-    <row r="2003" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2003" s="5"/>
-      <c r="B2003" s="5"/>
-      <c r="C2003" s="6"/>
-      <c r="D2003" s="5"/>
-      <c r="E2003" s="5"/>
-    </row>
-    <row r="2004" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2004" s="5"/>
-      <c r="B2004" s="5"/>
-      <c r="C2004" s="6"/>
-      <c r="D2004" s="5"/>
-      <c r="E2004" s="5"/>
-    </row>
-    <row r="2005" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2005" s="5"/>
-      <c r="B2005" s="5"/>
-      <c r="C2005" s="6"/>
-      <c r="D2005" s="5"/>
-      <c r="E2005" s="5"/>
-    </row>
-    <row r="2006" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2006" s="5"/>
-      <c r="B2006" s="5"/>
-      <c r="C2006" s="6"/>
-      <c r="D2006" s="5"/>
-      <c r="E2006" s="5"/>
-    </row>
-    <row r="2007" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2007" s="5"/>
-      <c r="B2007" s="5"/>
-      <c r="C2007" s="6"/>
-      <c r="D2007" s="5"/>
-      <c r="E2007" s="5"/>
-    </row>
-    <row r="2008" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2008" s="5"/>
-      <c r="B2008" s="5"/>
-      <c r="C2008" s="6"/>
-      <c r="D2008" s="5"/>
-      <c r="E2008" s="5"/>
-    </row>
-    <row r="2009" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2009" s="5"/>
-      <c r="B2009" s="5"/>
-      <c r="C2009" s="6"/>
-      <c r="D2009" s="5"/>
-      <c r="E2009" s="5"/>
-    </row>
-    <row r="2010" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2010" s="5"/>
-      <c r="B2010" s="5"/>
-      <c r="C2010" s="6"/>
-      <c r="D2010" s="5"/>
-      <c r="E2010" s="5"/>
-    </row>
-    <row r="2011" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2011" s="5"/>
-      <c r="B2011" s="5"/>
-      <c r="C2011" s="6"/>
-      <c r="D2011" s="5"/>
-      <c r="E2011" s="5"/>
-    </row>
-    <row r="2012" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2012" s="5"/>
-      <c r="B2012" s="5"/>
-      <c r="C2012" s="6"/>
-      <c r="D2012" s="5"/>
-      <c r="E2012" s="5"/>
-    </row>
-    <row r="2013" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2013" s="5"/>
-      <c r="B2013" s="5"/>
-      <c r="C2013" s="6"/>
-      <c r="D2013" s="5"/>
-      <c r="E2013" s="5"/>
-    </row>
-    <row r="2014" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2014" s="5"/>
-      <c r="B2014" s="5"/>
-      <c r="C2014" s="6"/>
-      <c r="D2014" s="5"/>
-      <c r="E2014" s="5"/>
-    </row>
-    <row r="2015" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2015" s="5"/>
-      <c r="B2015" s="5"/>
-      <c r="C2015" s="6"/>
-      <c r="D2015" s="5"/>
-      <c r="E2015" s="5"/>
-    </row>
-    <row r="2016" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2016" s="5"/>
-      <c r="B2016" s="5"/>
-      <c r="C2016" s="6"/>
-      <c r="D2016" s="5"/>
-      <c r="E2016" s="5"/>
-    </row>
-    <row r="2017" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2017" s="5"/>
-      <c r="B2017" s="5"/>
-      <c r="C2017" s="6"/>
-      <c r="D2017" s="5"/>
-      <c r="E2017" s="5"/>
-    </row>
-    <row r="2018" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2018" s="5"/>
-      <c r="B2018" s="5"/>
-      <c r="C2018" s="6"/>
-      <c r="D2018" s="5"/>
-      <c r="E2018" s="5"/>
-    </row>
-    <row r="2019" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2019" s="5"/>
-      <c r="B2019" s="5"/>
-      <c r="C2019" s="6"/>
-      <c r="D2019" s="5"/>
-      <c r="E2019" s="5"/>
-    </row>
-    <row r="2020" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2020" s="5"/>
-      <c r="B2020" s="5"/>
-      <c r="C2020" s="6"/>
-      <c r="D2020" s="5"/>
-      <c r="E2020" s="5"/>
-    </row>
-    <row r="2021" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2021" s="5"/>
-      <c r="B2021" s="5"/>
-      <c r="C2021" s="6"/>
-      <c r="D2021" s="5"/>
-      <c r="E2021" s="5"/>
-    </row>
-    <row r="2022" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2022" s="5"/>
-      <c r="B2022" s="5"/>
-      <c r="C2022" s="6"/>
-      <c r="D2022" s="5"/>
-      <c r="E2022" s="5"/>
-    </row>
-    <row r="2023" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2023" s="5"/>
-      <c r="B2023" s="5"/>
-      <c r="C2023" s="6"/>
-      <c r="D2023" s="5"/>
-      <c r="E2023" s="5"/>
-    </row>
-    <row r="2024" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2024" s="5"/>
-      <c r="B2024" s="5"/>
-      <c r="C2024" s="6"/>
-      <c r="D2024" s="5"/>
-      <c r="E2024" s="5"/>
-    </row>
-    <row r="2025" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2025" s="5"/>
-      <c r="B2025" s="5"/>
-      <c r="C2025" s="6"/>
-      <c r="D2025" s="5"/>
-      <c r="E2025" s="5"/>
-    </row>
-    <row r="2026" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2026" s="5"/>
-      <c r="B2026" s="5"/>
-      <c r="C2026" s="6"/>
-      <c r="D2026" s="5"/>
-      <c r="E2026" s="5"/>
-    </row>
-    <row r="2027" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2027" s="5"/>
-      <c r="B2027" s="5"/>
-      <c r="C2027" s="6"/>
-      <c r="D2027" s="5"/>
-      <c r="E2027" s="5"/>
-    </row>
-    <row r="2028" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2028" s="5"/>
-      <c r="B2028" s="5"/>
-      <c r="C2028" s="6"/>
-      <c r="D2028" s="5"/>
-      <c r="E2028" s="5"/>
-    </row>
-    <row r="2029" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2029" s="5"/>
-      <c r="B2029" s="5"/>
-      <c r="C2029" s="6"/>
-      <c r="D2029" s="5"/>
-      <c r="E2029" s="5"/>
-    </row>
-    <row r="2030" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2030" s="5"/>
-      <c r="B2030" s="5"/>
-      <c r="C2030" s="6"/>
-      <c r="D2030" s="5"/>
-      <c r="E2030" s="5"/>
-    </row>
-    <row r="2031" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2031" s="5"/>
-      <c r="B2031" s="5"/>
-      <c r="C2031" s="6"/>
-      <c r="D2031" s="5"/>
-      <c r="E2031" s="5"/>
-    </row>
-    <row r="2032" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2032" s="5"/>
-      <c r="B2032" s="5"/>
-      <c r="C2032" s="6"/>
-      <c r="D2032" s="5"/>
-      <c r="E2032" s="5"/>
-    </row>
-    <row r="2033" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2033" s="5"/>
-      <c r="B2033" s="5"/>
-      <c r="C2033" s="6"/>
-      <c r="D2033" s="5"/>
-      <c r="E2033" s="5"/>
-    </row>
-    <row r="2034" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2034" s="5"/>
-      <c r="B2034" s="5"/>
-      <c r="C2034" s="6"/>
-      <c r="D2034" s="5"/>
-      <c r="E2034" s="5"/>
-    </row>
-    <row r="2035" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2035" s="5"/>
-      <c r="B2035" s="5"/>
-      <c r="C2035" s="6"/>
-      <c r="D2035" s="5"/>
-      <c r="E2035" s="5"/>
-    </row>
-    <row r="2036" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2036" s="5"/>
-      <c r="B2036" s="5"/>
-      <c r="C2036" s="6"/>
-      <c r="D2036" s="5"/>
-      <c r="E2036" s="5"/>
-    </row>
-    <row r="2037" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2037" s="5"/>
-      <c r="B2037" s="5"/>
-      <c r="C2037" s="6"/>
-      <c r="D2037" s="5"/>
-      <c r="E2037" s="5"/>
-    </row>
-    <row r="2038" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2038" s="5"/>
-      <c r="B2038" s="5"/>
-      <c r="C2038" s="6"/>
-      <c r="D2038" s="5"/>
-      <c r="E2038" s="5"/>
-    </row>
-    <row r="2039" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2039" s="5"/>
-      <c r="B2039" s="5"/>
-      <c r="C2039" s="6"/>
-      <c r="D2039" s="5"/>
-      <c r="E2039" s="5"/>
-    </row>
-    <row r="2040" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2040" s="5"/>
-      <c r="B2040" s="5"/>
-      <c r="C2040" s="6"/>
-      <c r="D2040" s="5"/>
-      <c r="E2040" s="5"/>
-    </row>
-    <row r="2041" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2041" s="5"/>
-      <c r="B2041" s="5"/>
-      <c r="C2041" s="6"/>
-      <c r="D2041" s="5"/>
-      <c r="E2041" s="5"/>
-    </row>
-    <row r="2042" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2042" s="5"/>
-      <c r="B2042" s="5"/>
-      <c r="C2042" s="6"/>
-      <c r="D2042" s="5"/>
-      <c r="E2042" s="5"/>
-    </row>
-    <row r="2043" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2043" s="5"/>
-      <c r="B2043" s="5"/>
-      <c r="C2043" s="6"/>
-      <c r="D2043" s="5"/>
-      <c r="E2043" s="5"/>
-    </row>
-    <row r="2044" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2044" s="5"/>
-      <c r="B2044" s="5"/>
-      <c r="C2044" s="6"/>
-      <c r="D2044" s="5"/>
-      <c r="E2044" s="5"/>
-    </row>
-    <row r="2045" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2045" s="5"/>
-      <c r="B2045" s="5"/>
-      <c r="C2045" s="6"/>
-      <c r="D2045" s="5"/>
-      <c r="E2045" s="5"/>
-    </row>
-    <row r="2046" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2046" s="5"/>
-      <c r="B2046" s="5"/>
-      <c r="C2046" s="6"/>
-      <c r="D2046" s="5"/>
-      <c r="E2046" s="5"/>
-    </row>
-    <row r="2047" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2047" s="5"/>
-      <c r="B2047" s="5"/>
-      <c r="C2047" s="6"/>
-      <c r="D2047" s="5"/>
-      <c r="E2047" s="5"/>
-    </row>
-    <row r="2048" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2048" s="5"/>
-      <c r="B2048" s="5"/>
-      <c r="C2048" s="6"/>
-      <c r="D2048" s="5"/>
-      <c r="E2048" s="5"/>
-    </row>
-    <row r="2049" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2049" s="5"/>
-      <c r="B2049" s="5"/>
-      <c r="C2049" s="6"/>
-      <c r="D2049" s="5"/>
-      <c r="E2049" s="5"/>
-    </row>
-    <row r="2050" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2050" s="5"/>
-      <c r="B2050" s="5"/>
-      <c r="C2050" s="6"/>
-      <c r="D2050" s="5"/>
-      <c r="E2050" s="5"/>
-    </row>
-    <row r="2051" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2051" s="5"/>
-      <c r="B2051" s="5"/>
-      <c r="C2051" s="6"/>
-      <c r="D2051" s="5"/>
-      <c r="E2051" s="5"/>
-    </row>
-    <row r="2052" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2052" s="5"/>
-      <c r="B2052" s="5"/>
-      <c r="C2052" s="6"/>
-      <c r="D2052" s="5"/>
-      <c r="E2052" s="5"/>
-    </row>
-    <row r="2053" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2053" s="5"/>
-      <c r="B2053" s="5"/>
-      <c r="C2053" s="6"/>
-      <c r="D2053" s="5"/>
-      <c r="E2053" s="5"/>
-    </row>
-    <row r="2054" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2054" s="5"/>
-      <c r="B2054" s="5"/>
-      <c r="C2054" s="6"/>
-      <c r="D2054" s="5"/>
-      <c r="E2054" s="5"/>
-    </row>
-    <row r="2055" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2055" s="5"/>
-      <c r="B2055" s="5"/>
-      <c r="C2055" s="6"/>
-      <c r="D2055" s="5"/>
-      <c r="E2055" s="5"/>
-    </row>
-    <row r="2056" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2056" s="5"/>
-      <c r="B2056" s="5"/>
-      <c r="C2056" s="6"/>
-      <c r="D2056" s="5"/>
-      <c r="E2056" s="5"/>
-    </row>
-    <row r="2057" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2057" s="5"/>
-      <c r="B2057" s="5"/>
-      <c r="C2057" s="6"/>
-      <c r="D2057" s="5"/>
-      <c r="E2057" s="5"/>
-    </row>
-    <row r="2058" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2058" s="5"/>
-      <c r="B2058" s="5"/>
-      <c r="C2058" s="6"/>
-      <c r="D2058" s="5"/>
-      <c r="E2058" s="5"/>
-    </row>
-    <row r="2059" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2059" s="5"/>
-      <c r="B2059" s="5"/>
-      <c r="C2059" s="6"/>
-      <c r="D2059" s="5"/>
-      <c r="E2059" s="5"/>
-    </row>
-    <row r="2060" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2060" s="5"/>
-      <c r="B2060" s="5"/>
-      <c r="C2060" s="6"/>
-      <c r="D2060" s="5"/>
-      <c r="E2060" s="5"/>
-    </row>
-    <row r="2061" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2061" s="5"/>
-      <c r="B2061" s="5"/>
-      <c r="C2061" s="6"/>
-      <c r="D2061" s="5"/>
-      <c r="E2061" s="5"/>
-    </row>
-    <row r="2062" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2062" s="5"/>
-      <c r="B2062" s="5"/>
-      <c r="C2062" s="6"/>
-      <c r="D2062" s="5"/>
-      <c r="E2062" s="5"/>
-    </row>
-    <row r="2063" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2063" s="5"/>
-      <c r="B2063" s="5"/>
-      <c r="C2063" s="6"/>
-      <c r="D2063" s="5"/>
-      <c r="E2063" s="5"/>
-    </row>
-    <row r="2064" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2064" s="5"/>
-      <c r="B2064" s="5"/>
-      <c r="C2064" s="6"/>
-      <c r="D2064" s="5"/>
-      <c r="E2064" s="5"/>
-    </row>
-    <row r="2065" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2065" s="5"/>
-      <c r="B2065" s="5"/>
-      <c r="C2065" s="6"/>
-      <c r="D2065" s="5"/>
-      <c r="E2065" s="5"/>
-    </row>
-    <row r="2066" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2066" s="5"/>
-      <c r="B2066" s="5"/>
-      <c r="C2066" s="6"/>
-      <c r="D2066" s="5"/>
-      <c r="E2066" s="5"/>
-    </row>
-    <row r="2067" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2067" s="5"/>
-      <c r="B2067" s="5"/>
-      <c r="C2067" s="6"/>
-      <c r="D2067" s="5"/>
-      <c r="E2067" s="5"/>
-    </row>
-    <row r="2068" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2068" s="5"/>
-      <c r="B2068" s="5"/>
-      <c r="C2068" s="6"/>
-      <c r="D2068" s="5"/>
-      <c r="E2068" s="5"/>
-    </row>
-    <row r="2069" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2069" s="5"/>
-      <c r="B2069" s="5"/>
-      <c r="C2069" s="6"/>
-      <c r="D2069" s="5"/>
-      <c r="E2069" s="5"/>
-    </row>
-    <row r="2070" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2070" s="5"/>
-      <c r="B2070" s="5"/>
-      <c r="C2070" s="6"/>
-      <c r="D2070" s="5"/>
-      <c r="E2070" s="5"/>
-    </row>
-    <row r="2071" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2071" s="5"/>
-      <c r="B2071" s="5"/>
-      <c r="C2071" s="6"/>
-      <c r="D2071" s="5"/>
-      <c r="E2071" s="5"/>
-    </row>
-    <row r="2072" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2072" s="5"/>
-      <c r="B2072" s="5"/>
-      <c r="C2072" s="6"/>
-      <c r="D2072" s="5"/>
-      <c r="E2072" s="5"/>
-    </row>
-    <row r="2073" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2073" s="5"/>
-      <c r="B2073" s="5"/>
-      <c r="C2073" s="6"/>
-      <c r="D2073" s="5"/>
-      <c r="E2073" s="5"/>
-    </row>
-    <row r="2074" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2074" s="5"/>
-      <c r="B2074" s="5"/>
-      <c r="C2074" s="6"/>
-      <c r="D2074" s="5"/>
-      <c r="E2074" s="5"/>
-    </row>
-    <row r="2075" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2075" s="5"/>
-      <c r="B2075" s="5"/>
-      <c r="C2075" s="6"/>
-      <c r="D2075" s="5"/>
-      <c r="E2075" s="5"/>
-    </row>
-    <row r="2076" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2076" s="5"/>
-      <c r="B2076" s="5"/>
-      <c r="C2076" s="6"/>
-      <c r="D2076" s="5"/>
-      <c r="E2076" s="5"/>
-    </row>
-    <row r="2077" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2077" s="5"/>
-      <c r="B2077" s="5"/>
-      <c r="C2077" s="6"/>
-      <c r="D2077" s="5"/>
-      <c r="E2077" s="5"/>
-    </row>
-    <row r="2078" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2078" s="5"/>
-      <c r="B2078" s="5"/>
-      <c r="C2078" s="6"/>
-      <c r="D2078" s="5"/>
-      <c r="E2078" s="5"/>
-    </row>
-    <row r="2079" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2079" s="5"/>
-      <c r="B2079" s="5"/>
-      <c r="C2079" s="6"/>
-      <c r="D2079" s="5"/>
-      <c r="E2079" s="5"/>
-    </row>
-    <row r="2080" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2080" s="5"/>
-      <c r="B2080" s="5"/>
-      <c r="C2080" s="6"/>
-      <c r="D2080" s="5"/>
-      <c r="E2080" s="5"/>
-    </row>
-    <row r="2081" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2081" s="5"/>
-      <c r="B2081" s="5"/>
-      <c r="C2081" s="6"/>
-      <c r="D2081" s="5"/>
-      <c r="E2081" s="5"/>
-    </row>
-    <row r="2082" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2082" s="5"/>
-      <c r="B2082" s="5"/>
-      <c r="C2082" s="6"/>
-      <c r="D2082" s="5"/>
-      <c r="E2082" s="5"/>
-    </row>
-    <row r="2083" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2083" s="5"/>
-      <c r="B2083" s="5"/>
-      <c r="C2083" s="6"/>
-      <c r="D2083" s="5"/>
-      <c r="E2083" s="5"/>
-    </row>
-    <row r="2084" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2084" s="5"/>
-      <c r="B2084" s="5"/>
-      <c r="C2084" s="6"/>
-      <c r="D2084" s="5"/>
-      <c r="E2084" s="5"/>
-    </row>
-    <row r="2085" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2085" s="5"/>
-      <c r="B2085" s="5"/>
-      <c r="C2085" s="6"/>
-      <c r="D2085" s="5"/>
-      <c r="E2085" s="5"/>
-    </row>
-    <row r="2086" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2086" s="5"/>
-      <c r="B2086" s="5"/>
-      <c r="C2086" s="6"/>
-      <c r="D2086" s="5"/>
-      <c r="E2086" s="5"/>
-    </row>
-    <row r="2087" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2087" s="5"/>
-      <c r="B2087" s="5"/>
-      <c r="C2087" s="6"/>
-      <c r="D2087" s="5"/>
-      <c r="E2087" s="5"/>
-    </row>
-    <row r="2088" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2088" s="5"/>
-      <c r="B2088" s="5"/>
-      <c r="C2088" s="6"/>
-      <c r="D2088" s="5"/>
-      <c r="E2088" s="5"/>
-    </row>
-    <row r="2089" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2089" s="5"/>
-      <c r="B2089" s="5"/>
-      <c r="C2089" s="6"/>
-      <c r="D2089" s="5"/>
-      <c r="E2089" s="5"/>
-    </row>
-    <row r="2090" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2090" s="5"/>
-      <c r="B2090" s="5"/>
-      <c r="C2090" s="6"/>
-      <c r="D2090" s="5"/>
-      <c r="E2090" s="5"/>
-    </row>
-    <row r="2091" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2091" s="5"/>
-      <c r="B2091" s="5"/>
-      <c r="C2091" s="6"/>
-      <c r="D2091" s="5"/>
-      <c r="E2091" s="5"/>
-    </row>
-    <row r="2092" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2092" s="5"/>
-      <c r="B2092" s="5"/>
-      <c r="C2092" s="6"/>
-      <c r="D2092" s="5"/>
-      <c r="E2092" s="5"/>
-    </row>
-    <row r="2093" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2093" s="5"/>
-      <c r="B2093" s="5"/>
-      <c r="C2093" s="6"/>
-      <c r="D2093" s="5"/>
-      <c r="E2093" s="5"/>
-    </row>
-    <row r="2094" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2094" s="5"/>
-      <c r="B2094" s="5"/>
-      <c r="C2094" s="6"/>
-      <c r="D2094" s="5"/>
-      <c r="E2094" s="5"/>
-    </row>
-    <row r="2095" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2095" s="5"/>
-      <c r="B2095" s="5"/>
-      <c r="C2095" s="6"/>
-      <c r="D2095" s="5"/>
-      <c r="E2095" s="5"/>
-    </row>
-    <row r="2096" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2096" s="5"/>
-      <c r="B2096" s="5"/>
-      <c r="C2096" s="6"/>
-      <c r="D2096" s="5"/>
-      <c r="E2096" s="5"/>
-    </row>
-    <row r="2097" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2097" s="5"/>
-      <c r="B2097" s="5"/>
-      <c r="C2097" s="6"/>
-      <c r="D2097" s="5"/>
-      <c r="E2097" s="5"/>
-    </row>
-    <row r="2098" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2098" s="5"/>
-      <c r="B2098" s="5"/>
-      <c r="C2098" s="6"/>
-      <c r="D2098" s="5"/>
-      <c r="E2098" s="5"/>
-    </row>
-    <row r="2099" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2099" s="5"/>
-      <c r="B2099" s="5"/>
-      <c r="C2099" s="6"/>
-      <c r="D2099" s="5"/>
-      <c r="E2099" s="5"/>
-    </row>
-    <row r="2100" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2100" s="5"/>
-      <c r="B2100" s="5"/>
-      <c r="C2100" s="6"/>
-      <c r="D2100" s="5"/>
-      <c r="E2100" s="5"/>
-    </row>
-    <row r="2101" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2101" s="5"/>
-      <c r="B2101" s="5"/>
-      <c r="C2101" s="6"/>
-      <c r="D2101" s="5"/>
-      <c r="E2101" s="5"/>
-    </row>
-    <row r="2102" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2102" s="5"/>
-      <c r="B2102" s="5"/>
-      <c r="C2102" s="6"/>
-      <c r="D2102" s="5"/>
-      <c r="E2102" s="5"/>
-    </row>
-    <row r="2103" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2103" s="5"/>
-      <c r="B2103" s="5"/>
-      <c r="C2103" s="6"/>
-      <c r="D2103" s="5"/>
-      <c r="E2103" s="5"/>
-    </row>
-    <row r="2104" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2104" s="5"/>
-      <c r="B2104" s="5"/>
-      <c r="C2104" s="6"/>
-      <c r="D2104" s="5"/>
-      <c r="E2104" s="5"/>
-    </row>
-    <row r="2105" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2105" s="5"/>
-      <c r="B2105" s="5"/>
-      <c r="C2105" s="6"/>
-      <c r="D2105" s="5"/>
-      <c r="E2105" s="5"/>
-    </row>
-    <row r="2106" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2106" s="5"/>
-      <c r="B2106" s="5"/>
-      <c r="C2106" s="6"/>
-      <c r="D2106" s="5"/>
-      <c r="E2106" s="5"/>
-    </row>
-    <row r="2107" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2107" s="5"/>
-      <c r="B2107" s="5"/>
-      <c r="C2107" s="6"/>
-      <c r="D2107" s="5"/>
-      <c r="E2107" s="5"/>
-    </row>
-    <row r="2108" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2108" s="5"/>
-      <c r="B2108" s="5"/>
-      <c r="C2108" s="6"/>
-      <c r="D2108" s="5"/>
-      <c r="E2108" s="5"/>
-    </row>
-    <row r="2109" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2109" s="5"/>
-      <c r="B2109" s="5"/>
-      <c r="C2109" s="6"/>
-      <c r="D2109" s="5"/>
-      <c r="E2109" s="5"/>
-    </row>
-    <row r="2110" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2110" s="5"/>
-      <c r="B2110" s="5"/>
-      <c r="C2110" s="6"/>
-      <c r="D2110" s="5"/>
-      <c r="E2110" s="5"/>
-    </row>
-    <row r="2111" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2111" s="5"/>
-      <c r="B2111" s="5"/>
-      <c r="C2111" s="6"/>
-      <c r="D2111" s="5"/>
-      <c r="E2111" s="5"/>
-    </row>
-    <row r="2112" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2112" s="5"/>
-      <c r="B2112" s="5"/>
-      <c r="C2112" s="6"/>
-      <c r="D2112" s="5"/>
-      <c r="E2112" s="5"/>
-    </row>
-    <row r="2113" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2113" s="5"/>
-      <c r="B2113" s="5"/>
-      <c r="C2113" s="6"/>
-      <c r="D2113" s="5"/>
-      <c r="E2113" s="5"/>
-    </row>
-    <row r="2114" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2114" s="5"/>
-      <c r="B2114" s="5"/>
-      <c r="C2114" s="6"/>
-      <c r="D2114" s="5"/>
-      <c r="E2114" s="5"/>
-    </row>
-    <row r="2115" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2115" s="5"/>
-      <c r="B2115" s="5"/>
-      <c r="C2115" s="6"/>
-      <c r="D2115" s="5"/>
-      <c r="E2115" s="5"/>
-    </row>
-    <row r="2116" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2116" s="5"/>
-      <c r="B2116" s="5"/>
-      <c r="C2116" s="6"/>
-      <c r="D2116" s="5"/>
-      <c r="E2116" s="5"/>
-    </row>
-    <row r="2117" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2117" s="5"/>
-      <c r="B2117" s="5"/>
-      <c r="C2117" s="6"/>
-      <c r="D2117" s="5"/>
-      <c r="E2117" s="5"/>
-    </row>
-    <row r="2118" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2118" s="5"/>
-      <c r="B2118" s="5"/>
-      <c r="C2118" s="6"/>
-      <c r="D2118" s="5"/>
-      <c r="E2118" s="5"/>
-    </row>
-    <row r="2119" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2119" s="5"/>
-      <c r="B2119" s="5"/>
-      <c r="C2119" s="6"/>
-      <c r="D2119" s="5"/>
-      <c r="E2119" s="5"/>
-    </row>
-    <row r="2120" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2120" s="5"/>
-      <c r="B2120" s="5"/>
-      <c r="C2120" s="6"/>
-      <c r="D2120" s="5"/>
-      <c r="E2120" s="5"/>
-    </row>
-    <row r="2121" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2121" s="5"/>
-      <c r="B2121" s="5"/>
-      <c r="C2121" s="6"/>
-      <c r="D2121" s="5"/>
-      <c r="E2121" s="5"/>
-    </row>
-    <row r="2122" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2122" s="5"/>
-      <c r="B2122" s="5"/>
-      <c r="C2122" s="6"/>
-      <c r="D2122" s="5"/>
-      <c r="E2122" s="5"/>
-    </row>
-    <row r="2123" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2123" s="5"/>
-      <c r="B2123" s="5"/>
-      <c r="C2123" s="6"/>
-      <c r="D2123" s="5"/>
-      <c r="E2123" s="5"/>
-    </row>
-    <row r="2124" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2124" s="5"/>
-      <c r="B2124" s="5"/>
-      <c r="C2124" s="6"/>
-      <c r="D2124" s="5"/>
-      <c r="E2124" s="5"/>
-    </row>
-    <row r="2125" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2125" s="5"/>
-      <c r="B2125" s="5"/>
-      <c r="C2125" s="6"/>
-      <c r="D2125" s="5"/>
-      <c r="E2125" s="5"/>
-    </row>
-    <row r="2126" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2126" s="5"/>
-      <c r="B2126" s="5"/>
-      <c r="C2126" s="6"/>
-      <c r="D2126" s="5"/>
-      <c r="E2126" s="5"/>
-    </row>
-    <row r="2127" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2127" s="5"/>
-      <c r="B2127" s="5"/>
-      <c r="C2127" s="6"/>
-      <c r="D2127" s="5"/>
-      <c r="E2127" s="5"/>
-    </row>
-    <row r="2128" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2128" s="5"/>
-      <c r="B2128" s="5"/>
-      <c r="C2128" s="6"/>
-      <c r="D2128" s="5"/>
-      <c r="E2128" s="5"/>
-    </row>
-    <row r="2129" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2129" s="5"/>
-      <c r="B2129" s="5"/>
-      <c r="C2129" s="6"/>
-      <c r="D2129" s="5"/>
-      <c r="E2129" s="5"/>
-    </row>
-    <row r="2130" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2130" s="5"/>
-      <c r="B2130" s="5"/>
-      <c r="C2130" s="6"/>
-      <c r="D2130" s="5"/>
-      <c r="E2130" s="5"/>
-    </row>
-    <row r="2131" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2131" s="5"/>
-      <c r="B2131" s="5"/>
-      <c r="C2131" s="6"/>
-      <c r="D2131" s="5"/>
-      <c r="E2131" s="5"/>
-    </row>
-    <row r="2132" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2132" s="5"/>
-      <c r="B2132" s="5"/>
-      <c r="C2132" s="6"/>
-      <c r="D2132" s="5"/>
-      <c r="E2132" s="5"/>
-    </row>
-    <row r="2133" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2133" s="5"/>
-      <c r="B2133" s="5"/>
-      <c r="C2133" s="6"/>
-      <c r="D2133" s="5"/>
-      <c r="E2133" s="5"/>
-    </row>
-    <row r="2134" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2134" s="5"/>
-      <c r="B2134" s="5"/>
-      <c r="C2134" s="6"/>
-      <c r="D2134" s="5"/>
-      <c r="E2134" s="5"/>
-    </row>
-    <row r="2135" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2135" s="5"/>
-      <c r="B2135" s="5"/>
-      <c r="C2135" s="6"/>
-      <c r="D2135" s="5"/>
-      <c r="E2135" s="5"/>
-    </row>
-    <row r="2136" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2136" s="5"/>
-      <c r="B2136" s="5"/>
-      <c r="C2136" s="6"/>
-      <c r="D2136" s="5"/>
-      <c r="E2136" s="5"/>
-    </row>
-    <row r="2137" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2137" s="5"/>
-      <c r="B2137" s="5"/>
-      <c r="C2137" s="6"/>
-      <c r="D2137" s="5"/>
-      <c r="E2137" s="5"/>
-    </row>
-    <row r="2138" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2138" s="5"/>
-      <c r="B2138" s="5"/>
-      <c r="C2138" s="6"/>
-      <c r="D2138" s="5"/>
-      <c r="E2138" s="5"/>
-    </row>
-    <row r="2139" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2139" s="5"/>
-      <c r="B2139" s="5"/>
-      <c r="C2139" s="6"/>
-      <c r="D2139" s="5"/>
-      <c r="E2139" s="5"/>
-    </row>
-    <row r="2140" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2140" s="5"/>
-      <c r="B2140" s="5"/>
-      <c r="C2140" s="6"/>
-      <c r="D2140" s="5"/>
-      <c r="E2140" s="5"/>
-    </row>
-    <row r="2141" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2141" s="5"/>
-      <c r="B2141" s="5"/>
-      <c r="C2141" s="6"/>
-      <c r="D2141" s="5"/>
-      <c r="E2141" s="5"/>
-    </row>
-    <row r="2142" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2142" s="5"/>
-      <c r="B2142" s="5"/>
-      <c r="C2142" s="6"/>
-      <c r="D2142" s="5"/>
-      <c r="E2142" s="5"/>
-    </row>
-    <row r="2143" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2143" s="5"/>
-      <c r="B2143" s="5"/>
-      <c r="C2143" s="6"/>
-      <c r="D2143" s="5"/>
-      <c r="E2143" s="5"/>
-    </row>
-    <row r="2144" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2144" s="5"/>
-      <c r="B2144" s="5"/>
-      <c r="C2144" s="6"/>
-      <c r="D2144" s="5"/>
-      <c r="E2144" s="5"/>
-    </row>
-    <row r="2145" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2145" s="5"/>
-      <c r="B2145" s="5"/>
-      <c r="C2145" s="6"/>
-      <c r="D2145" s="5"/>
-      <c r="E2145" s="5"/>
-    </row>
-    <row r="2146" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2146" s="5"/>
-      <c r="B2146" s="5"/>
-      <c r="C2146" s="6"/>
-      <c r="D2146" s="5"/>
-      <c r="E2146" s="5"/>
-    </row>
-    <row r="2147" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2147" s="5"/>
-      <c r="B2147" s="5"/>
-      <c r="C2147" s="6"/>
-      <c r="D2147" s="5"/>
-      <c r="E2147" s="5"/>
-    </row>
-    <row r="2148" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2148" s="5"/>
-      <c r="B2148" s="5"/>
-      <c r="C2148" s="6"/>
-      <c r="D2148" s="5"/>
-      <c r="E2148" s="5"/>
-    </row>
-    <row r="2149" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2149" s="5"/>
-      <c r="B2149" s="5"/>
-      <c r="C2149" s="6"/>
-      <c r="D2149" s="5"/>
-      <c r="E2149" s="5"/>
-    </row>
-    <row r="2150" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2150" s="5"/>
-      <c r="B2150" s="5"/>
-      <c r="C2150" s="6"/>
-      <c r="D2150" s="5"/>
-      <c r="E2150" s="5"/>
-    </row>
-    <row r="2151" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2151" s="5"/>
-      <c r="B2151" s="5"/>
-      <c r="C2151" s="6"/>
-      <c r="D2151" s="5"/>
-      <c r="E2151" s="5"/>
-    </row>
-    <row r="2152" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2152" s="5"/>
-      <c r="B2152" s="5"/>
-      <c r="C2152" s="6"/>
-      <c r="D2152" s="5"/>
-      <c r="E2152" s="5"/>
-    </row>
-    <row r="2153" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2153" s="5"/>
-      <c r="B2153" s="5"/>
-      <c r="C2153" s="6"/>
-      <c r="D2153" s="5"/>
-      <c r="E2153" s="5"/>
-    </row>
-    <row r="2154" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2154" s="5"/>
-      <c r="B2154" s="5"/>
-      <c r="C2154" s="6"/>
-      <c r="D2154" s="5"/>
-      <c r="E2154" s="5"/>
-    </row>
-    <row r="2155" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2155" s="5"/>
-      <c r="B2155" s="5"/>
-      <c r="C2155" s="6"/>
-      <c r="D2155" s="5"/>
-      <c r="E2155" s="5"/>
-    </row>
-    <row r="2156" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2156" s="5"/>
-      <c r="B2156" s="5"/>
-      <c r="C2156" s="6"/>
-      <c r="D2156" s="5"/>
-      <c r="E2156" s="5"/>
-    </row>
-    <row r="2157" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2157" s="5"/>
-      <c r="B2157" s="5"/>
-      <c r="C2157" s="6"/>
-      <c r="D2157" s="5"/>
-      <c r="E2157" s="5"/>
-    </row>
-    <row r="2158" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2158" s="5"/>
-      <c r="B2158" s="5"/>
-      <c r="C2158" s="6"/>
-      <c r="D2158" s="5"/>
-      <c r="E2158" s="5"/>
-    </row>
-    <row r="2159" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2159" s="5"/>
-      <c r="B2159" s="5"/>
-      <c r="C2159" s="6"/>
-      <c r="D2159" s="5"/>
-      <c r="E2159" s="5"/>
-    </row>
-    <row r="2160" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2160" s="5"/>
-      <c r="B2160" s="5"/>
-      <c r="C2160" s="6"/>
-      <c r="D2160" s="5"/>
-      <c r="E2160" s="5"/>
-    </row>
-    <row r="2161" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2161" s="5"/>
-      <c r="B2161" s="5"/>
-      <c r="C2161" s="6"/>
-      <c r="D2161" s="5"/>
-      <c r="E2161" s="5"/>
-    </row>
-    <row r="2162" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2162" s="5"/>
-      <c r="B2162" s="5"/>
-      <c r="C2162" s="6"/>
-      <c r="D2162" s="5"/>
-      <c r="E2162" s="5"/>
-    </row>
-    <row r="2163" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2163" s="5"/>
-      <c r="B2163" s="5"/>
-      <c r="C2163" s="6"/>
-      <c r="D2163" s="5"/>
-      <c r="E2163" s="5"/>
-    </row>
-    <row r="2164" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2164" s="5"/>
-      <c r="B2164" s="5"/>
-      <c r="C2164" s="6"/>
-      <c r="D2164" s="5"/>
-      <c r="E2164" s="5"/>
-    </row>
-    <row r="2165" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2165" s="5"/>
-      <c r="B2165" s="5"/>
-      <c r="C2165" s="6"/>
-      <c r="D2165" s="5"/>
-      <c r="E2165" s="5"/>
-    </row>
-    <row r="2166" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2166" s="5"/>
-      <c r="B2166" s="5"/>
-      <c r="C2166" s="6"/>
-      <c r="D2166" s="5"/>
-      <c r="E2166" s="5"/>
-    </row>
-    <row r="2167" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2167" s="5"/>
-      <c r="B2167" s="5"/>
-      <c r="C2167" s="6"/>
-      <c r="D2167" s="5"/>
-      <c r="E2167" s="5"/>
-    </row>
-    <row r="2168" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2168" s="5"/>
-      <c r="B2168" s="5"/>
-      <c r="C2168" s="6"/>
-      <c r="D2168" s="5"/>
-      <c r="E2168" s="5"/>
-    </row>
-    <row r="2169" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2169" s="5"/>
-      <c r="B2169" s="5"/>
-      <c r="C2169" s="6"/>
-      <c r="D2169" s="5"/>
-      <c r="E2169" s="5"/>
-    </row>
-    <row r="2170" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2170" s="5"/>
-      <c r="B2170" s="5"/>
-      <c r="C2170" s="6"/>
-      <c r="D2170" s="5"/>
-      <c r="E2170" s="5"/>
-    </row>
-    <row r="2171" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2171" s="5"/>
-      <c r="B2171" s="5"/>
-      <c r="C2171" s="6"/>
-      <c r="D2171" s="5"/>
-      <c r="E2171" s="5"/>
-    </row>
-    <row r="2172" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2172" s="5"/>
-      <c r="B2172" s="5"/>
-      <c r="C2172" s="6"/>
-      <c r="D2172" s="5"/>
-      <c r="E2172" s="5"/>
-    </row>
-    <row r="2173" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2173" s="5"/>
-      <c r="B2173" s="5"/>
-      <c r="C2173" s="6"/>
-      <c r="D2173" s="5"/>
-      <c r="E2173" s="5"/>
-    </row>
-    <row r="2174" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2174" s="5"/>
-      <c r="B2174" s="5"/>
-      <c r="C2174" s="6"/>
-      <c r="D2174" s="5"/>
-      <c r="E2174" s="5"/>
-    </row>
-    <row r="2175" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2175" s="5"/>
-      <c r="B2175" s="5"/>
-      <c r="C2175" s="6"/>
-      <c r="D2175" s="5"/>
-      <c r="E2175" s="5"/>
-    </row>
-    <row r="2176" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2176" s="5"/>
-      <c r="B2176" s="5"/>
-      <c r="C2176" s="6"/>
-      <c r="D2176" s="5"/>
-      <c r="E2176" s="5"/>
-    </row>
-    <row r="2177" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2177" s="5"/>
-      <c r="B2177" s="5"/>
-      <c r="C2177" s="6"/>
-      <c r="D2177" s="5"/>
-      <c r="E2177" s="5"/>
-    </row>
-    <row r="2178" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2178" s="5"/>
-      <c r="B2178" s="5"/>
-      <c r="C2178" s="6"/>
-      <c r="D2178" s="5"/>
-      <c r="E2178" s="5"/>
-    </row>
-    <row r="2179" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2179" s="5"/>
-      <c r="B2179" s="5"/>
-      <c r="C2179" s="6"/>
-      <c r="D2179" s="5"/>
-      <c r="E2179" s="5"/>
-    </row>
-    <row r="2180" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2180" s="5"/>
-      <c r="B2180" s="5"/>
-      <c r="C2180" s="6"/>
-      <c r="D2180" s="5"/>
-      <c r="E2180" s="5"/>
-    </row>
-    <row r="2181" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2181" s="5"/>
-      <c r="B2181" s="5"/>
-      <c r="C2181" s="6"/>
-      <c r="D2181" s="5"/>
-      <c r="E2181" s="5"/>
-    </row>
-    <row r="2182" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2182" s="5"/>
-      <c r="B2182" s="5"/>
-      <c r="C2182" s="6"/>
-      <c r="D2182" s="5"/>
-      <c r="E2182" s="5"/>
-    </row>
-    <row r="2183" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2183" s="5"/>
-      <c r="B2183" s="5"/>
-      <c r="C2183" s="6"/>
-      <c r="D2183" s="5"/>
-      <c r="E2183" s="5"/>
-    </row>
-    <row r="2184" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2184" s="5"/>
-      <c r="B2184" s="5"/>
-      <c r="C2184" s="6"/>
-      <c r="D2184" s="5"/>
-      <c r="E2184" s="5"/>
-    </row>
-    <row r="2185" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2185" s="5"/>
-      <c r="B2185" s="5"/>
-      <c r="C2185" s="6"/>
-      <c r="D2185" s="5"/>
-      <c r="E2185" s="5"/>
-    </row>
-    <row r="2186" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2186" s="5"/>
-      <c r="B2186" s="5"/>
-      <c r="C2186" s="6"/>
-      <c r="D2186" s="5"/>
-      <c r="E2186" s="5"/>
-    </row>
-    <row r="2187" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2187" s="5"/>
-      <c r="B2187" s="5"/>
-      <c r="C2187" s="6"/>
-      <c r="D2187" s="5"/>
-      <c r="E2187" s="5"/>
-    </row>
-    <row r="2188" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2188" s="5"/>
-      <c r="B2188" s="5"/>
-      <c r="C2188" s="6"/>
-      <c r="D2188" s="5"/>
-      <c r="E2188" s="5"/>
-    </row>
-    <row r="2189" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2189" s="5"/>
-      <c r="B2189" s="5"/>
-      <c r="C2189" s="6"/>
-      <c r="D2189" s="5"/>
-      <c r="E2189" s="5"/>
+      <c r="A2001" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2001" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2001" s="6">
+        <f t="shared" si="31"/>
+        <v>62201856035</v>
+      </c>
+      <c r="D2001" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2001" s="5" t="s">
+        <v>87</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>